<commit_message>
Nhat Linh : update ThongKeNVBanHang JPanel
</commit_message>
<xml_diff>
--- a/DuLieuThongKe/ThongKeMatHangBanChayNam2023.xlsx
+++ b/DuLieuThongKe/ThongKeMatHangBanChayNam2023.xlsx
@@ -62,19 +62,19 @@
     <t>Top 3</t>
   </si>
   <si>
+    <t>HH0013S</t>
+  </si>
+  <si>
+    <t>Thắt lưng da</t>
+  </si>
+  <si>
+    <t>Top 4</t>
+  </si>
+  <si>
     <t>HH0011M</t>
   </si>
   <si>
     <t>Mũ lưỡi trai</t>
-  </si>
-  <si>
-    <t>Top 4</t>
-  </si>
-  <si>
-    <t>HH0013S</t>
-  </si>
-  <si>
-    <t>Thắt lưng da</t>
   </si>
 </sst>
 </file>
@@ -230,13 +230,13 @@
         <v>1.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>52000.0</v>
+        <v>265000.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>110.0</v>
+        <v>342.0</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>321.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="5">
@@ -256,13 +256,13 @@
         <v>1.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>0.0</v>
+        <v>52000.0</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>342.0</v>
+        <v>110.0</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>13.0</v>
+        <v>321.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>